<commit_message>
Add Day 1 dialog
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED2B8AD-06A0-4A8D-8A8C-282359C91F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2A7E47-E233-4DCB-905A-7EFD0868B6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
   <sheets>
     <sheet name="part" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,10 +57,6 @@
   </si>
   <si>
     <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>audio</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -430,27 +426,125 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>母亲</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>我</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>妹妹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>女生</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>第一部分</t>
+    <t>第一天上午</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>这是一行测试文本</t>
+    <t>旁白</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>诶，咋了娘。</t>
+  </si>
+  <si>
+    <t>李志强</t>
+  </si>
+  <si>
+    <t>赵秀红</t>
+  </si>
+  <si>
+    <t>跟娘去把水稻插上，猪给喂咯。</t>
+  </si>
+  <si>
+    <t>好嘞。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一天田地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>娘，今天我想到处转转。</t>
+  </si>
+  <si>
+    <t>去吧，不过晚上五点记得回家吃饭。</t>
+  </si>
+  <si>
+    <t>第一天选择提前回家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天想在外面转转，暂时还不想回去。</t>
+  </si>
+  <si>
+    <t>第一天傍晚回家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爹这是咋了？！</t>
+  </si>
+  <si>
+    <t>唉……今天搬砖头的时候，一个没留神，砸着胳膊了。不过没事，就蹭破点皮。</t>
+  </si>
+  <si>
+    <t>哦这样啊，那还好。</t>
+  </si>
+  <si>
+    <t>来来来，来吃饭了。今天有好喝的蘑菇汤。</t>
+  </si>
+  <si>
+    <t>李春苗</t>
+  </si>
+  <si>
+    <t>哎，干嘛呢。你哥都还没坐下。</t>
+  </si>
+  <si>
+    <t>……</t>
+  </si>
+  <si>
+    <t>谢谢哥！</t>
+  </si>
+  <si>
+    <t>第一天晚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（估计晚上汤喝多了，有点想上厕所……）</t>
+  </si>
+  <si>
+    <t>哎，秀红，你说我这工作没了，志强的学费咋办啊……</t>
+  </si>
+  <si>
+    <t>要我看，就别让他上学了吧。我觉得读书也没啥用啊，还不如在家里多干点活。</t>
+  </si>
+  <si>
+    <t>这是什么话，读了书，有了知识，将来才能出息啊！</t>
+  </si>
+  <si>
+    <t>可你看现在，咱家哪还出得起学费啊。你手折了，看医生不也得花钱吗？</t>
+  </si>
+  <si>
+    <t>哎，说的也是啊。可，可我怎么跟他说呢。志强那孩子，那么喜欢读书，我也一直答应他，会供他上学……</t>
+  </si>
+  <si>
+    <t>我来跟他说就是了。志强孝顺，能理解你的。行了，睡吧。</t>
+  </si>
+  <si>
+    <t>蘑菇汤~！（伸勺子舀汤）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>……</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没事儿妈，妹想喝汤就喝呗。（走过来坐下，给春苗舀汤）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1990年春，南沟村。\n"志强，志强……"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -994,17 +1088,17 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1012,99 +1106,123 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -1124,40 +1242,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="97" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1165,102 +1283,472 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="J3" s="8"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J4" s="8"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="J5" s="8"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="J6" s="8"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="J7" s="8"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="J8" s="8"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J9" s="8"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="J13" s="8"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="J14" s="11"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" autoFilter="0"/>
@@ -1270,6 +1758,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1283,7 +1772,7 @@
           <x14:formula1>
             <xm:f>part!$A$2:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>B4:B1048576 B2 C3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1299,41 +1788,43 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="I2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1344,7 +1835,7 @@
       <c r="L3" s="17"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1355,7 +1846,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1366,7 +1857,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1377,7 +1868,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1388,7 +1879,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1399,7 +1890,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1410,7 +1901,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1421,7 +1912,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1432,7 +1923,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1443,7 +1934,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1454,7 +1945,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1465,7 +1956,7 @@
       <c r="L14" s="17"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1476,7 +1967,7 @@
       <c r="L15" s="17"/>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1487,7 +1978,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1498,7 +1989,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1509,793 +2000,793 @@
       <c r="L18" s="20"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -2334,18 +2825,18 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2353,30 +2844,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="9"/>
@@ -2384,12 +2875,12 @@
       <c r="K3" s="9"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="9"/>
@@ -2397,12 +2888,12 @@
       <c r="K4" s="9"/>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
@@ -2410,12 +2901,12 @@
       <c r="K5" s="9"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="9"/>
@@ -2423,56 +2914,62 @@
       <c r="K6" s="9"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="H7" s="8"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H8" s="8"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="10"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H9" s="8"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H10" s="8"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H11" s="8"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H12" s="8"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>

</xml_diff>

<commit_message>
Finished normal dialog showing
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2A7E47-E233-4DCB-905A-7EFD0868B6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2D35FF-A5DD-4522-B045-C1FA902B079D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="character" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">character!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">character!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dialog!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">part!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">selection!$A$1:$C$1</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,10 +57,6 @@
   </si>
   <si>
     <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>drawing</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -116,198 +112,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">	name：这一part的名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">简介：
-该表用于存放对话
-表头：
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <family val="2"/>
-        <charset val="2"/>
-      </rPr>
-      <t></t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	id：递增编号
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <family val="2"/>
-        <charset val="2"/>
-      </rPr>
-      <t></t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	partid：这一对话属于的part的id（介绍见part表）
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <family val="2"/>
-        <charset val="2"/>
-      </rPr>
-      <t></t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	speaker：讲话的人的id
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <family val="2"/>
-        <charset val="2"/>
-      </rPr>
-      <t></t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	content：讲话的内容
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <family val="2"/>
-        <charset val="2"/>
-      </rPr>
-      <t></t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	audio：对应的音频相对路径，若无请留空</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">简介：
-该表用于存放游戏角色（包括主角）
-表头：
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <family val="2"/>
-        <charset val="2"/>
-      </rPr>
-      <t></t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	id：递增编号
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <family val="2"/>
-        <charset val="2"/>
-      </rPr>
-      <t></t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	name：人物名
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <family val="2"/>
-        <charset val="2"/>
-      </rPr>
-      <t></t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	drawing：立绘相对路径</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -545,6 +349,154 @@
   </si>
   <si>
     <t>normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">简介：
+该表用于存放游戏角色（包括主角）
+表头：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <family val="2"/>
+        <charset val="2"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	id：递增编号
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <family val="2"/>
+        <charset val="2"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	name：人物名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">简介：
+该表用于存放对话
+表头：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <family val="2"/>
+        <charset val="2"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	id：递增编号
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <family val="2"/>
+        <charset val="2"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	partid：这一对话属于的part的id（介绍见part表）
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <family val="2"/>
+        <charset val="2"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	speaker：讲话的人的id
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <family val="2"/>
+        <charset val="2"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	content：讲话的内容</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1111,10 +1063,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1126,7 +1078,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
@@ -1139,7 +1091,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
@@ -1152,7 +1104,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
@@ -1165,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
@@ -1245,7 +1197,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1263,13 +1215,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1286,13 +1238,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -1310,10 +1262,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="9"/>
@@ -1332,10 +1284,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="9"/>
@@ -1354,10 +1306,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="9"/>
@@ -1376,10 +1328,10 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="9"/>
@@ -1398,10 +1350,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="9"/>
@@ -1420,10 +1372,10 @@
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="9"/>
@@ -1442,10 +1394,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="9"/>
@@ -1464,10 +1416,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
@@ -1486,10 +1438,10 @@
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
@@ -1508,10 +1460,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9"/>
@@ -1530,10 +1482,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="9"/>
@@ -1552,10 +1504,10 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="12"/>
@@ -1574,10 +1526,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1591,10 +1543,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1608,10 +1560,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1625,10 +1577,10 @@
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1642,10 +1594,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1659,10 +1611,10 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1676,10 +1628,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1693,10 +1645,10 @@
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1710,10 +1662,10 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1727,10 +1679,10 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1744,10 +1696,10 @@
         <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1802,13 +1754,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1817,7 +1769,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="I2" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
@@ -2822,165 +2774,161 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8261C956-EF23-4F69-8888-584A7AE13E73}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.875" style="3"/>
+    <col min="3" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="10"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H8" s="8"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="10"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H9" s="8"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="10"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H10" s="8"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H11" s="8"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H12" s="8"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H13" s="8"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="11"/>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
+      <c r="K14" s="13"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" autoFilter="0"/>
-  <autoFilter ref="A1:C1" xr:uid="{8261C956-EF23-4F69-8888-584A7AE13E73}"/>
+  <autoFilter ref="A1:B1" xr:uid="{8261C956-EF23-4F69-8888-584A7AE13E73}"/>
   <mergeCells count="1">
-    <mergeCell ref="H2:L14"/>
+    <mergeCell ref="G2:K14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add fullscreen dialog tween
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2D35FF-A5DD-4522-B045-C1FA902B079D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03E159B-4EDF-4F44-8197-118C7707927F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
@@ -340,10 +340,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1990年春，南沟村。\n"志强，志强……"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>emotion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -497,6 +493,10 @@
       </rPr>
       <t xml:space="preserve">	content：讲话的内容</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1990年春，南沟村。\n"志强，志强……"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1197,7 +1197,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1221,7 +1221,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1238,13 +1238,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -1262,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
@@ -1284,7 +1284,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>17</v>
@@ -1306,7 +1306,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
@@ -1328,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>20</v>
@@ -1350,7 +1350,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>21</v>
@@ -1372,7 +1372,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>23</v>
@@ -1394,7 +1394,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>25</v>
@@ -1416,7 +1416,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>26</v>
@@ -1438,7 +1438,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>27</v>
@@ -1460,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>28</v>
@@ -1482,7 +1482,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>41</v>
@@ -1504,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>30</v>
@@ -1526,7 +1526,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>42</v>
@@ -1543,7 +1543,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>43</v>
@@ -1560,7 +1560,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>32</v>
@@ -1577,7 +1577,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>34</v>
@@ -1594,7 +1594,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>35</v>
@@ -1611,7 +1611,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>36</v>
@@ -1628,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>37</v>
@@ -1645,7 +1645,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>38</v>
@@ -1662,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>39</v>
@@ -1679,7 +1679,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>40</v>
@@ -1696,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>31</v>
@@ -2803,7 +2803,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>

</xml_diff>

<commit_message>
Add unknown speaker dialog
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03E159B-4EDF-4F44-8197-118C7707927F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BED84A5-090B-4171-93D3-CC47EE185D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -496,7 +496,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1990年春，南沟村。\n"志强，志强……"</t>
+    <t>1990年春，南沟村。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>志强，志强……</t>
+  </si>
+  <si>
+    <t>unknown</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1194,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1235,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>45</v>
@@ -1259,13 +1266,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="9"/>
@@ -1281,13 +1288,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="9"/>
@@ -1303,13 +1310,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="9"/>
@@ -1322,7 +1329,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
         <v>3</v>
@@ -1331,7 +1338,7 @@
         <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="9"/>
@@ -1347,13 +1354,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="9"/>
@@ -1366,16 +1373,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="9"/>
@@ -1388,7 +1395,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
@@ -1397,7 +1404,7 @@
         <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="9"/>
@@ -1413,13 +1420,13 @@
         <v>4</v>
       </c>
       <c r="C10" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
@@ -1435,13 +1442,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
@@ -1457,13 +1464,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9"/>
@@ -1479,13 +1486,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="9"/>
@@ -1501,13 +1508,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="12"/>
@@ -1523,13 +1530,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1540,13 +1547,13 @@
         <v>4</v>
       </c>
       <c r="C16" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1557,13 +1564,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1571,16 +1578,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1591,13 +1598,13 @@
         <v>5</v>
       </c>
       <c r="C19" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1608,13 +1615,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1625,13 +1632,13 @@
         <v>5</v>
       </c>
       <c r="C21" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1642,13 +1649,13 @@
         <v>5</v>
       </c>
       <c r="C22" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1659,13 +1666,13 @@
         <v>5</v>
       </c>
       <c r="C23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1676,13 +1683,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1693,12 +1700,29 @@
         <v>5</v>
       </c>
       <c r="C25" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>5</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1714,17 +1738,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{12D47E0F-5466-428A-A28E-E1ACBFF036E8}">
+          <x14:formula1>
+            <xm:f>part!$A$2:$A$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2 C4 B5:B1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DF41E39-455D-45E0-B4E4-591C933514BF}">
           <x14:formula1>
             <xm:f>character!$A$2:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{12D47E0F-5466-428A-A28E-E1ACBFF036E8}">
-          <x14:formula1>
-            <xm:f>part!$A$2:$A$100</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4:B1048576 B2 C3</xm:sqref>
+          <xm:sqref>C2 C4:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2777,7 +2801,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2864,7 +2888,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -2876,6 +2900,12 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>

</xml_diff>

<commit_message>
Finished Dialog selection and load dialogs of day 2
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBC9E8F-9F93-42FC-B7E7-BDB222E96411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D1AAEE-0457-402D-963F-19C255FAF974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="96">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -226,10 +226,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>父亲</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>第一天上午</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -505,6 +501,159 @@
   <si>
     <t>郑敏</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二天早</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李建国</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>志强啊，今天集市开张了，你爹我手伤了不方便，你帮忙把你娘织的帕子拿去卖呗。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>……好。</t>
+  </si>
+  <si>
+    <t>第二天到达集市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不知走了多久，终于到了集市。集市上人来人往，热闹得很。</t>
+  </si>
+  <si>
+    <t>先逛一逛吧，现在没什么心情叫卖。</t>
+  </si>
+  <si>
+    <t>NPC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瞧一瞧，看一看了，物美价廉，童叟无欺呀。</t>
+  </si>
+  <si>
+    <t>叫卖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该怎么叫卖呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花帕子，一毛钱两条，嘿嘿！;浙江温州江南帕子厂倒闭啦，黄鹤老板跟他小姨子跑啦，帕子通通大甩卖啦。;俺娘做的花帕子，用完皮都展开了，这是可以说的吗？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>……没有人买诶</t>
+  </si>
+  <si>
+    <t>转眼到了傍晚，大家都纷纷收摊回家了，可帕子还是没卖出去。</t>
+  </si>
+  <si>
+    <t>诶，你这帕子挺不错的啊，多少钱？</t>
+  </si>
+  <si>
+    <t>一条帕子五分钱。</t>
+  </si>
+  <si>
+    <t>嗨，便宜点成不？这都快收摊了。</t>
+  </si>
+  <si>
+    <t>哎，真不行，这已经是最低价了，俺娘亲手做的，质量可好着呢。;成成成，算你四分钱吧。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S2A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S2B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>那我不买了吧。</t>
+  </si>
+  <si>
+    <t>诶，别走啊，便宜算你得了。;不买就不买，才几个钱呢，真小气。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S3A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S3B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>那就三分钱吧。</t>
+  </si>
+  <si>
+    <t>谢谢，谢谢您。</t>
+  </si>
+  <si>
+    <t>怎么说话的呢，小兔崽子，怪不得卖不出东西。（骂骂咧咧地走）</t>
+  </si>
+  <si>
+    <t>小伙子爽快哈。</t>
+  </si>
+  <si>
+    <t>第二天回家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>志强，回来了，来，过来坐。今天卖了多少帕子呀？</t>
+  </si>
+  <si>
+    <t>就一张。四分钱。</t>
+  </si>
+  <si>
+    <t>怎么才卖一张呀？</t>
+  </si>
+  <si>
+    <t>哎孩子第一次卖，没经验嘛。</t>
+  </si>
+  <si>
+    <t>……对不起。</t>
+  </si>
+  <si>
+    <t>行吧，没事，下次赶集再卖也成。不过这收入实在是太少了，哎……志强，你爹他手伤的还挺重的，他老板不让他去上班了。</t>
+  </si>
+  <si>
+    <t>（面露难色）</t>
+  </si>
+  <si>
+    <t>娘，昨晚我路过你们房外，听见了。</t>
+  </si>
+  <si>
+    <t>那你这上学的事儿，先放一放成吗？</t>
+  </si>
+  <si>
+    <t>娘，我理解家里有困难。可是这学，我是一定得上的。至于学费，我可以自己想办法挣。</t>
+  </si>
+  <si>
+    <t>你这孩子……你爸伤了，我织帕子也挣不了几个钱，苗苗又还小，咱家，就指望你了呀。你出去打工挣的钱，要是拿去交了学费，家里可怎么办呀？</t>
+  </si>
+  <si>
+    <t>算了，秀红。孩子想上学，就让他上吧。</t>
+  </si>
+  <si>
+    <t>那谁来养家呀？</t>
+  </si>
+  <si>
+    <t>我……我再想想办法。</t>
+  </si>
+  <si>
+    <t>娘，你别生气。我会养家的。</t>
+  </si>
+  <si>
+    <t>娘就知道，你最孝顺了。最近郑家的饭馆好像在招伙计，你去看看？</t>
+  </si>
+  <si>
+    <t>好的，娘，我明儿就去。</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1196,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1070,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>5</v>
@@ -1085,7 +1234,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
@@ -1098,7 +1247,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
@@ -1111,7 +1260,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
@@ -1124,7 +1273,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
@@ -1133,6 +1282,12 @@
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -1140,6 +1295,12 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -1147,6 +1308,12 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -1154,6 +1321,12 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -1161,6 +1334,12 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -1168,6 +1347,12 @@
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -1175,6 +1360,12 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1182,6 +1373,12 @@
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -1201,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1228,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1245,13 +1442,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -1269,10 +1466,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="9"/>
@@ -1291,10 +1488,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="9"/>
@@ -1313,10 +1510,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="9"/>
@@ -1335,10 +1532,10 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="9"/>
@@ -1357,10 +1554,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="9"/>
@@ -1379,10 +1576,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="9"/>
@@ -1401,10 +1598,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="9"/>
@@ -1423,10 +1620,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
@@ -1445,10 +1642,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
@@ -1467,10 +1664,10 @@
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9"/>
@@ -1489,10 +1686,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="9"/>
@@ -1511,10 +1708,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="12"/>
@@ -1533,10 +1730,10 @@
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1550,10 +1747,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1567,10 +1764,10 @@
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1584,10 +1781,10 @@
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1601,10 +1798,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1618,10 +1815,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1635,10 +1832,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1652,10 +1849,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1669,10 +1866,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1686,10 +1883,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1703,10 +1900,10 @@
         <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1720,10 +1917,588 @@
         <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>7</v>
+      </c>
+      <c r="C29" s="2">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>7</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>7</v>
+      </c>
+      <c r="C31" s="2">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>8</v>
+      </c>
+      <c r="C32" s="2">
+        <v>7</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>8</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>8</v>
+      </c>
+      <c r="C34" s="2">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>8</v>
+      </c>
+      <c r="C35" s="2">
+        <v>8</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>8</v>
+      </c>
+      <c r="C37" s="2">
+        <v>8</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>9</v>
+      </c>
+      <c r="C38" s="2">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>11</v>
+      </c>
+      <c r="C39" s="2">
+        <v>8</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2">
+        <v>11</v>
+      </c>
+      <c r="C40" s="2">
+        <v>3</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>12</v>
+      </c>
+      <c r="C41" s="2">
+        <v>8</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2">
+        <v>10</v>
+      </c>
+      <c r="C42" s="2">
+        <v>8</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2">
+        <v>13</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2">
+        <v>13</v>
+      </c>
+      <c r="C44" s="2">
+        <v>3</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>30</v>
+      <c r="B45" s="2">
+        <v>13</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2">
+        <v>13</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2">
+        <v>13</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2">
+        <v>13</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2">
+        <v>13</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2">
+        <v>13</v>
+      </c>
+      <c r="C50" s="2">
+        <v>3</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2">
+        <v>13</v>
+      </c>
+      <c r="C51" s="2">
+        <v>2</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2">
+        <v>13</v>
+      </c>
+      <c r="C52" s="2">
+        <v>3</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2">
+        <v>13</v>
+      </c>
+      <c r="C53" s="2">
+        <v>2</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2">
+        <v>13</v>
+      </c>
+      <c r="C54" s="2">
+        <v>3</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2">
+        <v>13</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2">
+        <v>13</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2">
+        <v>13</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2">
+        <v>13</v>
+      </c>
+      <c r="C58" s="2">
+        <v>3</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2">
+        <v>13</v>
+      </c>
+      <c r="C59" s="2">
+        <v>2</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2">
+        <v>13</v>
+      </c>
+      <c r="C60" s="2">
+        <v>3</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1761,7 +2536,7 @@
   <dimension ref="A1:M150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1788,9 +2563,15 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="I2" s="5" t="s">
         <v>9</v>
@@ -1801,9 +2582,15 @@
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="I3" s="16"/>
       <c r="J3" s="17"/>
@@ -1812,9 +2599,15 @@
       <c r="M3" s="18"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="I4" s="16"/>
       <c r="J4" s="17"/>
@@ -2801,7 +3594,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2824,10 +3617,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -2839,7 +3632,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
@@ -2852,7 +3645,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
@@ -2865,7 +3658,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
@@ -2878,7 +3671,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
@@ -2891,7 +3684,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
@@ -2904,7 +3697,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
@@ -2913,6 +3706,12 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>

</xml_diff>

<commit_message>
Finished money screening during dialog; Update dice images
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E266FAC7-5523-4028-ACD7-058A46243E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444E5981-15C9-401B-B4DE-53103135C781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="110">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -558,10 +558,6 @@
     <t>嗨，便宜点成不？这都快收摊了。</t>
   </si>
   <si>
-    <t>哎，真不行，这已经是最低价了，俺娘亲手做的，质量可好着呢。;成成成，算你四分钱吧。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>S2B</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -677,6 +673,42 @@
   </si>
   <si>
     <t>开始甄别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有问题了！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>真币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>假币，未识破</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>假币，且识破</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看起来应该是真钱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这是假币，本次收入为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你怎么能用假币买东西呢！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这是一张真钱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哎，真不行，这已经是最低价了，俺娘亲手做的，质量可好着呢。（骰子点数+技能点数大于10时成功）;成成成，算你四分钱吧。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1217,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B08BA5-9D33-400C-B73F-DB35ECCAFF73}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1349,7 +1381,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
@@ -1362,7 +1394,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
@@ -1375,7 +1407,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
@@ -1388,7 +1420,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
@@ -1401,7 +1433,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
@@ -1414,7 +1446,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1422,7 +1454,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1438,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2164,7 +2220,7 @@
         <v>43</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2181,7 +2237,7 @@
         <v>43</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2198,7 +2254,7 @@
         <v>43</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2215,7 +2271,7 @@
         <v>43</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2232,7 +2288,7 @@
         <v>43</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2249,7 +2305,7 @@
         <v>43</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2266,7 +2322,7 @@
         <v>43</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2283,7 +2339,7 @@
         <v>43</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2300,7 +2356,7 @@
         <v>43</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2317,7 +2373,7 @@
         <v>43</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2334,7 +2390,7 @@
         <v>43</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -2351,7 +2407,7 @@
         <v>43</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -2368,7 +2424,7 @@
         <v>43</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2385,7 +2441,7 @@
         <v>43</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2402,7 +2458,7 @@
         <v>43</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2419,7 +2475,7 @@
         <v>43</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2453,7 +2509,7 @@
         <v>43</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2470,7 +2526,7 @@
         <v>43</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2487,7 +2543,7 @@
         <v>43</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2504,7 +2560,7 @@
         <v>43</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2521,7 +2577,7 @@
         <v>43</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2538,7 +2594,7 @@
         <v>43</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2555,7 +2611,7 @@
         <v>43</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2572,7 +2628,7 @@
         <v>43</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2589,7 +2645,7 @@
         <v>43</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2606,7 +2662,75 @@
         <v>43</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>101</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="B65" s="2">
+        <v>15</v>
+      </c>
+      <c r="C65" s="2">
+        <v>7</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>65</v>
+      </c>
+      <c r="B66" s="2">
+        <v>16</v>
+      </c>
+      <c r="C66" s="2">
+        <v>3</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" s="2">
+        <v>17</v>
+      </c>
+      <c r="C67" s="2">
+        <v>7</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2">
+        <v>18</v>
+      </c>
+      <c r="C68" s="2">
+        <v>3</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2625,13 +2749,13 @@
           <x14:formula1>
             <xm:f>part!$A$2:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>B2 C4 B5:B1048576</xm:sqref>
+          <xm:sqref>B2 C4 B65:B1048576 B5:B63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DF41E39-455D-45E0-B4E4-591C933514BF}">
           <x14:formula1>
             <xm:f>character!$A$2:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>C2 C4:C1048576</xm:sqref>
+          <xm:sqref>C2 C65:C1048576 C4:C63</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2644,7 +2768,7 @@
   <dimension ref="A1:M150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2697,7 +2821,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="D3" s="2"/>
       <c r="I3" s="16"/>
@@ -2714,7 +2838,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="2"/>
       <c r="I4" s="16"/>
@@ -2724,9 +2848,15 @@
       <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>64</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="I5" s="16"/>
       <c r="J5" s="17"/>
@@ -3818,7 +3948,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>

</xml_diff>

<commit_message>
Change skill point dialog images; Finished Going market coin collect and animation
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444E5981-15C9-401B-B4DE-53103135C781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE2334A-E881-4A6E-B446-5EEC75ABA396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
   <sheets>
     <sheet name="part" sheetId="1" r:id="rId1"/>
@@ -583,9 +583,6 @@
     <t>谢谢，谢谢您。</t>
   </si>
   <si>
-    <t>怎么说话的呢，小兔崽子，怪不得卖不出东西。（骂骂咧咧地走）</t>
-  </si>
-  <si>
     <t>小伙子爽快哈。</t>
   </si>
   <si>
@@ -709,6 +706,10 @@
   </si>
   <si>
     <t>哎，真不行，这已经是最低价了，俺娘亲手做的，质量可好着呢。（骰子点数+技能点数大于10时成功）;成成成，算你四分钱吧。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怎么说话的呢，怪不得卖不出东西。（骂骂咧咧地走）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1255,14 +1256,14 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.875" style="3"/>
+    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1285,7 +1286,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1298,7 +1299,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1311,7 +1312,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1324,7 +1325,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1337,7 +1338,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1350,7 +1351,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1363,7 +1364,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1376,12 +1377,12 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
@@ -1389,7 +1390,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1402,7 +1403,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1415,7 +1416,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1428,12 +1429,12 @@
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
@@ -1441,44 +1442,44 @@
       <c r="J14" s="12"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1496,21 +1497,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="97" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.875" style="3"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1551,7 +1552,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1573,7 +1574,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1595,7 +1596,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1617,7 +1618,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1639,7 +1640,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1661,7 +1662,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1683,7 +1684,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1705,7 +1706,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1727,7 +1728,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1749,7 +1750,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1771,7 +1772,7 @@
       <c r="M12" s="9"/>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1793,7 +1794,7 @@
       <c r="M13" s="9"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1815,7 +1816,7 @@
       <c r="M14" s="12"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1832,7 +1833,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1849,7 +1850,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1900,7 +1901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1917,7 +1918,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1934,7 +1935,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1968,7 +1969,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2002,7 +2003,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2036,7 +2037,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2087,7 +2088,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2172,7 +2173,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2240,7 +2241,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2257,7 +2258,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2271,10 +2272,10 @@
         <v>43</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2288,10 +2289,10 @@
         <v>43</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2305,10 +2306,10 @@
         <v>43</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2322,10 +2323,10 @@
         <v>43</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2339,10 +2340,10 @@
         <v>43</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2356,10 +2357,10 @@
         <v>43</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2373,10 +2374,10 @@
         <v>43</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2390,10 +2391,10 @@
         <v>43</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2407,10 +2408,10 @@
         <v>43</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2424,10 +2425,10 @@
         <v>43</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2441,10 +2442,10 @@
         <v>43</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2458,10 +2459,10 @@
         <v>43</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2475,10 +2476,10 @@
         <v>43</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2495,7 +2496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2509,10 +2510,10 @@
         <v>43</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2526,10 +2527,10 @@
         <v>43</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2543,10 +2544,10 @@
         <v>43</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2560,10 +2561,10 @@
         <v>43</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2577,10 +2578,10 @@
         <v>43</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2594,10 +2595,10 @@
         <v>43</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2611,10 +2612,10 @@
         <v>43</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2628,10 +2629,10 @@
         <v>43</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2645,10 +2646,10 @@
         <v>43</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2662,10 +2663,10 @@
         <v>43</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2679,10 +2680,10 @@
         <v>43</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2696,10 +2697,10 @@
         <v>43</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2713,10 +2714,10 @@
         <v>43</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2730,7 +2731,7 @@
         <v>43</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2767,20 +2768,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E10AC76-C302-4BE2-85A6-ECB2A2FFE8EF}">
   <dimension ref="A1:M150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.875" style="3"/>
+    <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2794,7 +2795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2813,7 +2814,7 @@
       <c r="L2" s="14"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2821,7 +2822,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" s="2"/>
       <c r="I3" s="16"/>
@@ -2830,7 +2831,7 @@
       <c r="L3" s="17"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2847,7 +2848,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2"/>
       <c r="I5" s="16"/>
@@ -2864,7 +2865,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2875,7 +2876,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2886,7 +2887,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2897,7 +2898,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2908,7 +2909,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2919,7 +2920,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2930,7 +2931,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2941,7 +2942,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2952,7 +2953,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2963,7 +2964,7 @@
       <c r="L14" s="17"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2974,7 +2975,7 @@
       <c r="L15" s="17"/>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2985,7 +2986,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2996,7 +2997,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3007,793 +3008,793 @@
       <c r="L18" s="20"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3835,14 +3836,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.875" style="3"/>
+    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3850,7 +3851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3865,7 +3866,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3878,7 +3879,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3891,7 +3892,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3904,7 +3905,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3917,7 +3918,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3930,7 +3931,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3943,12 +3944,12 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>
@@ -3956,35 +3957,35 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>

</xml_diff>

<commit_message>
Add character collider and scene colliders
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE2334A-E881-4A6E-B446-5EEC75ABA396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8858FE0E-DF9F-4F50-9F72-5452D76E215A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">character!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dialog!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dialog!$A$1:$E$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">part!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">selection!$A$1:$C$1</definedName>
   </definedNames>
@@ -555,9 +555,6 @@
     <t>一条帕子五分钱。</t>
   </si>
   <si>
-    <t>嗨，便宜点成不？这都快收摊了。</t>
-  </si>
-  <si>
     <t>S2B</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -709,7 +706,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>怎么说话的呢，怪不得卖不出东西。（骂骂咧咧地走）</t>
+    <t>便宜点成不？这都快收摊了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怎么说话的呢，怪不得卖不出东西。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1382,7 +1383,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
@@ -1395,7 +1396,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
@@ -1408,7 +1409,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
@@ -1421,7 +1422,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
@@ -1434,7 +1435,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
@@ -1447,7 +1448,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1455,7 +1456,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1463,7 +1464,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1471,7 +1472,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1479,7 +1480,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1497,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2204,7 +2205,7 @@
         <v>43</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2221,7 +2222,7 @@
         <v>43</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2238,7 +2239,7 @@
         <v>43</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2255,7 +2256,7 @@
         <v>43</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2289,7 +2290,7 @@
         <v>43</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2306,7 +2307,7 @@
         <v>43</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2323,7 +2324,7 @@
         <v>43</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2340,7 +2341,7 @@
         <v>43</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2357,7 +2358,7 @@
         <v>43</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,7 +2375,7 @@
         <v>43</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2391,7 +2392,7 @@
         <v>43</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2408,7 +2409,7 @@
         <v>43</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2425,7 +2426,7 @@
         <v>43</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2442,7 +2443,7 @@
         <v>43</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2459,7 +2460,7 @@
         <v>43</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2476,7 +2477,7 @@
         <v>43</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2510,7 +2511,7 @@
         <v>43</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2527,7 +2528,7 @@
         <v>43</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2544,7 +2545,7 @@
         <v>43</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2561,7 +2562,7 @@
         <v>43</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,7 +2579,7 @@
         <v>43</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2595,7 +2596,7 @@
         <v>43</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2612,7 +2613,7 @@
         <v>43</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2629,7 +2630,7 @@
         <v>43</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2646,7 +2647,7 @@
         <v>43</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2663,7 +2664,7 @@
         <v>43</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,7 +2681,7 @@
         <v>43</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2697,7 +2698,7 @@
         <v>43</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,7 +2715,7 @@
         <v>43</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2731,12 +2732,12 @@
         <v>43</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" autoFilter="0"/>
-  <autoFilter ref="A1:E1" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}"/>
+  <autoFilter ref="A1:E68" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}"/>
   <mergeCells count="1">
     <mergeCell ref="J2:N14"/>
   </mergeCells>
@@ -2822,7 +2823,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="2"/>
       <c r="I3" s="16"/>
@@ -2839,7 +2840,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="2"/>
       <c r="I4" s="16"/>
@@ -2856,7 +2857,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="2"/>
       <c r="I5" s="16"/>
@@ -3949,7 +3950,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>

</xml_diff>

<commit_message>
Add beginner's guide and sort dialog data by ID before use
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8858FE0E-DF9F-4F50-9F72-5452D76E215A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FCF567-957D-477E-AF1C-6C3C6A30F283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
   <sheets>
     <sheet name="part" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="121">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -712,6 +712,43 @@
   <si>
     <t>怎么说话的呢，怪不得卖不出东西。</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>农田新手教程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鼠标左键点击右上角背包图标打开物品栏</t>
+  </si>
+  <si>
+    <t>左键点击物品栏中的种子</t>
+  </si>
+  <si>
+    <t>右键点击要种下的地块（只有左边第一列可种，其他田地需要花钱开垦）</t>
+  </si>
+  <si>
+    <t>种植成功！随时间推移，种植的作物将会成熟，收割后可以出售，是非常重要的经济来源哦~</t>
+  </si>
+  <si>
+    <t>去集市小游戏教程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去集市路途遥远，需要玩一个小小的游戏，AD左右移动，W键跳跃，收集金币可转化成你的资产哦！</t>
+  </si>
+  <si>
+    <t>在集市情绪提示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>右边是情绪条，你现在的情绪值有点低，可以通过购买喜欢的物品来提高情绪值。情绪值若太低，有一定几率做出不理智事件哦！</t>
+  </si>
+  <si>
+    <t>正式开始的说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每天至少要上交家里1块钱 剩余的钱存起来当做学费 需要在九月开学之前攒够学费</t>
   </si>
 </sst>
 </file>
@@ -1251,20 +1288,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B08BA5-9D33-400C-B73F-DB35ECCAFF73}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1287,7 +1324,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1300,7 +1337,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1313,7 +1350,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1326,7 +1363,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1339,7 +1376,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1352,7 +1389,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1365,7 +1402,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1378,7 +1415,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1391,7 +1428,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1404,7 +1441,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1417,7 +1454,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1430,7 +1467,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1443,7 +1480,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1451,7 +1488,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1459,7 +1496,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1467,7 +1504,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1475,12 +1512,44 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1496,23 +1565,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" style="2" customWidth="1"/>
     <col min="5" max="5" width="97" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="6" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1529,7 +1598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1553,7 +1622,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1575,7 +1644,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1597,7 +1666,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1619,7 +1688,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1641,7 +1710,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1663,7 +1732,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1685,7 +1754,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1707,7 +1776,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1729,7 +1798,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1751,7 +1820,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1773,7 +1842,7 @@
       <c r="M12" s="9"/>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1795,7 +1864,7 @@
       <c r="M13" s="9"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1817,7 +1886,7 @@
       <c r="M14" s="12"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1834,7 +1903,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1851,7 +1920,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1868,7 +1937,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1885,7 +1954,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1902,7 +1971,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1919,7 +1988,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1936,7 +2005,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1953,7 +2022,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1970,7 +2039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1987,7 +2056,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2004,7 +2073,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2021,7 +2090,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2038,7 +2107,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2055,7 +2124,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2072,7 +2141,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2089,7 +2158,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2106,7 +2175,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2123,7 +2192,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2140,7 +2209,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2157,7 +2226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2174,7 +2243,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2191,7 +2260,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2208,7 +2277,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2225,7 +2294,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2242,7 +2311,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2259,7 +2328,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2276,7 +2345,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2293,7 +2362,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2310,7 +2379,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2327,7 +2396,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2344,7 +2413,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2361,7 +2430,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2378,7 +2447,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2395,7 +2464,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2412,7 +2481,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2429,7 +2498,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2446,7 +2515,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2463,7 +2532,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2480,7 +2549,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2497,7 +2566,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2514,7 +2583,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2531,7 +2600,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2548,7 +2617,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2565,7 +2634,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2582,7 +2651,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2599,7 +2668,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2616,7 +2685,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2633,7 +2702,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2650,7 +2719,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2667,7 +2736,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2684,7 +2753,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2701,7 +2770,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2718,7 +2787,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2733,6 +2802,125 @@
       </c>
       <c r="E68" s="2" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2">
+        <v>19</v>
+      </c>
+      <c r="C69" s="2">
+        <v>7</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>69</v>
+      </c>
+      <c r="B70" s="2">
+        <v>19</v>
+      </c>
+      <c r="C70" s="2">
+        <v>7</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>70</v>
+      </c>
+      <c r="B71" s="2">
+        <v>19</v>
+      </c>
+      <c r="C71" s="2">
+        <v>7</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2">
+        <v>19</v>
+      </c>
+      <c r="C72" s="2">
+        <v>7</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
+        <v>72</v>
+      </c>
+      <c r="B73" s="2">
+        <v>20</v>
+      </c>
+      <c r="C73" s="2">
+        <v>7</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="B74" s="2">
+        <v>21</v>
+      </c>
+      <c r="C74" s="2">
+        <v>7</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2">
+        <v>22</v>
+      </c>
+      <c r="C75" s="2">
+        <v>7</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2773,16 +2961,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="5" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2796,7 +2984,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2815,7 +3003,7 @@
       <c r="L2" s="14"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2832,7 +3020,7 @@
       <c r="L3" s="17"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2849,7 +3037,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2866,7 +3054,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2877,7 +3065,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2888,7 +3076,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2899,7 +3087,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2910,7 +3098,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2921,7 +3109,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2932,7 +3120,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2943,7 +3131,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2954,7 +3142,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2965,7 +3153,7 @@
       <c r="L14" s="17"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2976,7 +3164,7 @@
       <c r="L15" s="17"/>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2987,7 +3175,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2998,7 +3186,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3009,793 +3197,793 @@
       <c r="L18" s="20"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3837,14 +4025,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3852,7 +4040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3867,7 +4055,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3880,7 +4068,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3893,7 +4081,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3906,7 +4094,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3919,7 +4107,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3932,7 +4120,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3945,7 +4133,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3958,35 +4146,35 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>

</xml_diff>

<commit_message>
Removed beginner's guide from dialog system
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FCF567-957D-477E-AF1C-6C3C6A30F283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAF12F1-378E-412D-ADA6-D589C69DE830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
   <sheets>
     <sheet name="part" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="110">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -712,43 +712,6 @@
   <si>
     <t>怎么说话的呢，怪不得卖不出东西。</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>农田新手教程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>鼠标左键点击右上角背包图标打开物品栏</t>
-  </si>
-  <si>
-    <t>左键点击物品栏中的种子</t>
-  </si>
-  <si>
-    <t>右键点击要种下的地块（只有左边第一列可种，其他田地需要花钱开垦）</t>
-  </si>
-  <si>
-    <t>种植成功！随时间推移，种植的作物将会成熟，收割后可以出售，是非常重要的经济来源哦~</t>
-  </si>
-  <si>
-    <t>去集市小游戏教程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>去集市路途遥远，需要玩一个小小的游戏，AD左右移动，W键跳跃，收集金币可转化成你的资产哦！</t>
-  </si>
-  <si>
-    <t>在集市情绪提示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>右边是情绪条，你现在的情绪值有点低，可以通过购买喜欢的物品来提高情绪值。情绪值若太低，有一定几率做出不理智事件哦！</t>
-  </si>
-  <si>
-    <t>正式开始的说明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每天至少要上交家里1块钱 剩余的钱存起来当做学费 需要在九月开学之前攒够学费</t>
   </si>
 </sst>
 </file>
@@ -1288,20 +1251,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B08BA5-9D33-400C-B73F-DB35ECCAFF73}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="A20:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.875" style="3"/>
+    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1309,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1324,7 +1287,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1337,7 +1300,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1350,7 +1313,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1363,7 +1326,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1376,7 +1339,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1389,7 +1352,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1402,7 +1365,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1415,7 +1378,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1428,7 +1391,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1441,7 +1404,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1454,7 +1417,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1467,7 +1430,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1480,7 +1443,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1488,7 +1451,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1496,7 +1459,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1504,7 +1467,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1512,44 +1475,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1560,28 +1491,29 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E75" sqref="A69:E75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="97" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.875" style="3"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1622,7 +1554,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1644,7 +1576,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1666,7 +1598,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1688,7 +1620,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1710,7 +1642,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1732,7 +1664,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1754,7 +1686,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1776,7 +1708,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1798,7 +1730,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1820,7 +1752,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1842,7 +1774,7 @@
       <c r="M12" s="9"/>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1864,7 +1796,7 @@
       <c r="M13" s="9"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1886,7 +1818,7 @@
       <c r="M14" s="12"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1903,7 +1835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1920,7 +1852,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1937,7 +1869,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1954,7 +1886,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1971,7 +1903,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1988,7 +1920,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2005,7 +1937,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2022,7 +1954,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2039,7 +1971,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2056,7 +1988,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2073,7 +2005,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2090,7 +2022,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2107,7 +2039,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2124,7 +2056,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2141,7 +2073,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2158,7 +2090,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2175,7 +2107,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2192,7 +2124,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2209,7 +2141,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2226,7 +2158,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2243,7 +2175,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2260,7 +2192,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2277,7 +2209,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2294,7 +2226,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2311,7 +2243,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2328,7 +2260,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2345,7 +2277,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2362,7 +2294,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2379,7 +2311,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2396,7 +2328,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2413,7 +2345,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2430,7 +2362,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2447,7 +2379,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2464,7 +2396,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2481,7 +2413,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2498,7 +2430,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2515,7 +2447,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2532,7 +2464,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2549,7 +2481,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2566,7 +2498,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2583,7 +2515,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2600,7 +2532,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2617,7 +2549,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2634,7 +2566,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2651,7 +2583,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2668,7 +2600,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2685,7 +2617,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2702,7 +2634,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2719,7 +2651,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2736,7 +2668,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2753,7 +2685,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2770,7 +2702,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2787,7 +2719,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2802,125 +2734,6 @@
       </c>
       <c r="E68" s="2" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="2">
-        <v>68</v>
-      </c>
-      <c r="B69" s="2">
-        <v>19</v>
-      </c>
-      <c r="C69" s="2">
-        <v>7</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="2">
-        <v>69</v>
-      </c>
-      <c r="B70" s="2">
-        <v>19</v>
-      </c>
-      <c r="C70" s="2">
-        <v>7</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="2">
-        <v>70</v>
-      </c>
-      <c r="B71" s="2">
-        <v>19</v>
-      </c>
-      <c r="C71" s="2">
-        <v>7</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="2">
-        <v>71</v>
-      </c>
-      <c r="B72" s="2">
-        <v>19</v>
-      </c>
-      <c r="C72" s="2">
-        <v>7</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="2">
-        <v>72</v>
-      </c>
-      <c r="B73" s="2">
-        <v>20</v>
-      </c>
-      <c r="C73" s="2">
-        <v>7</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="2">
-        <v>73</v>
-      </c>
-      <c r="B74" s="2">
-        <v>21</v>
-      </c>
-      <c r="C74" s="2">
-        <v>7</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="2">
-        <v>74</v>
-      </c>
-      <c r="B75" s="2">
-        <v>22</v>
-      </c>
-      <c r="C75" s="2">
-        <v>7</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2961,16 +2774,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.875" style="3"/>
+    <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2984,7 +2797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3003,7 +2816,7 @@
       <c r="L2" s="14"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3020,7 +2833,7 @@
       <c r="L3" s="17"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3037,7 +2850,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3054,7 +2867,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3065,7 +2878,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3076,7 +2889,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3087,7 +2900,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3098,7 +2911,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3109,7 +2922,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3120,7 +2933,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3131,7 +2944,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3142,7 +2955,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3153,7 +2966,7 @@
       <c r="L14" s="17"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3164,7 +2977,7 @@
       <c r="L15" s="17"/>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3175,7 +2988,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3186,7 +2999,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3197,793 +3010,793 @@
       <c r="L18" s="20"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -4025,14 +3838,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.875" style="3"/>
+    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4040,7 +3853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4055,7 +3868,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4068,7 +3881,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4081,7 +3894,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4094,7 +3907,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4107,7 +3920,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4120,7 +3933,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4133,7 +3946,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4146,35 +3959,35 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>

</xml_diff>

<commit_message>
Add dialog show when arrived at market
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAF12F1-378E-412D-ADA6-D589C69DE830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4059753-38FC-4CA3-B3FC-45A151EE01C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
   <sheets>
     <sheet name="part" sheetId="1" r:id="rId1"/>
@@ -1253,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B08BA5-9D33-400C-B73F-DB35ECCAFF73}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="A20:B23"/>
     </sheetView>
   </sheetViews>
@@ -1499,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E75" sqref="A69:E75"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2098,7 @@
         <v>7</v>
       </c>
       <c r="C31" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Add emotion recovery hint; Fixed item price problem
	modified:   Assets/Editors/Data/GameData.xlsx
	modified:   Assets/Scenes/Market.unity
	modified:   Assets/Scripts/Inventory/ShopInventory.cs
	modified:   Assets/Scripts/Item/EmotionRecoveryItem.cs
	modified:   Assets/Scripts/Item/Item.cs
	modified:   UserSettings/EditorUserSettings.asset
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4059753-38FC-4CA3-B3FC-45A151EE01C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45178405-7EC8-4450-96C3-CD91E75826F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
   <sheets>
     <sheet name="part" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="112">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -711,6 +711,14 @@
   </si>
   <si>
     <t>怎么说话的呢，怪不得卖不出东西。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>购买物品后</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>心情好多了！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1251,20 +1259,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B08BA5-9D33-400C-B73F-DB35ECCAFF73}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="A20:B23"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1287,7 +1295,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1300,7 +1308,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1313,7 +1321,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1326,7 +1334,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1339,7 +1347,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1352,7 +1360,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1365,7 +1373,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1378,7 +1386,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1391,7 +1399,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1404,7 +1412,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1417,7 +1425,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1430,7 +1438,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1443,7 +1451,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1451,7 +1459,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1459,7 +1467,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1467,7 +1475,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1475,12 +1483,20 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1497,23 +1513,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" style="2" customWidth="1"/>
     <col min="5" max="5" width="97" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="6" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1530,7 +1546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1554,7 +1570,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1576,7 +1592,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1598,7 +1614,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1620,7 +1636,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1642,7 +1658,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1664,7 +1680,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1686,7 +1702,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1708,7 +1724,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1730,7 +1746,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1752,7 +1768,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1774,7 +1790,7 @@
       <c r="M12" s="9"/>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1796,7 +1812,7 @@
       <c r="M13" s="9"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1818,7 +1834,7 @@
       <c r="M14" s="12"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1835,7 +1851,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1852,7 +1868,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1869,7 +1885,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1886,7 +1902,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1903,7 +1919,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1920,7 +1936,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1937,7 +1953,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1954,7 +1970,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1971,7 +1987,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1988,7 +2004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2005,7 +2021,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2022,7 +2038,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2039,7 +2055,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2056,7 +2072,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2073,7 +2089,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2090,7 +2106,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2107,7 +2123,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2124,7 +2140,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2141,7 +2157,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2158,7 +2174,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2175,7 +2191,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2192,7 +2208,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2209,7 +2225,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2226,7 +2242,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2243,7 +2259,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2260,7 +2276,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2277,7 +2293,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2294,7 +2310,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2311,7 +2327,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2328,7 +2344,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2345,7 +2361,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2362,7 +2378,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2379,7 +2395,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2396,7 +2412,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2413,7 +2429,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2430,7 +2446,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2447,7 +2463,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2464,7 +2480,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2481,7 +2497,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2498,7 +2514,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2515,7 +2531,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2532,7 +2548,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2549,7 +2565,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2566,7 +2582,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2583,7 +2599,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2600,7 +2616,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2617,7 +2633,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2634,7 +2650,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2651,7 +2667,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2668,7 +2684,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2685,7 +2701,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2702,7 +2718,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2719,7 +2735,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2734,6 +2750,23 @@
       </c>
       <c r="E68" s="2" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2">
+        <v>19</v>
+      </c>
+      <c r="C69" s="2">
+        <v>3</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2774,16 +2807,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="5" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2797,7 +2830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2816,7 +2849,7 @@
       <c r="L2" s="14"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2833,7 +2866,7 @@
       <c r="L3" s="17"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2850,7 +2883,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2867,7 +2900,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2878,7 +2911,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2889,7 +2922,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2900,7 +2933,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2911,7 +2944,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2922,7 +2955,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2933,7 +2966,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2944,7 +2977,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2955,7 +2988,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2966,7 +2999,7 @@
       <c r="L14" s="17"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2977,7 +3010,7 @@
       <c r="L15" s="17"/>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2988,7 +3021,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2999,7 +3032,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3010,793 +3043,793 @@
       <c r="L18" s="20"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3838,14 +3871,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3853,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3868,7 +3901,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3881,7 +3914,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3894,7 +3927,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3907,7 +3940,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3920,7 +3953,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3933,7 +3966,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3946,7 +3979,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3959,35 +3992,35 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>

</xml_diff>

<commit_message>
Fixed dialog order at home
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45178405-7EC8-4450-96C3-CD91E75826F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6910DC8D-C8B7-4AF5-9DCE-45273E954ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
   <sheets>
     <sheet name="part" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">character!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dialog!$A$1:$E$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dialog!$A$1:$E$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">part!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">selection!$A$1:$C$1</definedName>
   </definedNames>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="113">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -243,9 +243,6 @@
     <t>赵秀红</t>
   </si>
   <si>
-    <t>跟娘去把水稻插上，猪给喂咯。</t>
-  </si>
-  <si>
     <t>好嘞。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -293,10 +290,6 @@
   </si>
   <si>
     <t>谢谢哥！</t>
-  </si>
-  <si>
-    <t>第一天晚</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>（估计晚上汤喝多了，有点想上厕所……）</t>
@@ -503,10 +496,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>第二天早</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>李建国</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -719,6 +708,22 @@
   </si>
   <si>
     <t>心情好多了！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑屏切换夜晚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（晚上）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（第二天早）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跟娘去把水稻插上，猪给喂咯。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1259,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B08BA5-9D33-400C-B73F-DB35ECCAFF73}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1300,7 +1305,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
@@ -1313,7 +1318,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
@@ -1326,7 +1331,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
@@ -1335,12 +1340,6 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -1348,12 +1347,6 @@
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -1365,7 +1358,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
@@ -1378,7 +1371,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>
@@ -1391,7 +1384,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
@@ -1404,7 +1397,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
@@ -1417,7 +1410,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
@@ -1430,7 +1423,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
@@ -1443,7 +1436,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
@@ -1456,7 +1449,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1464,7 +1457,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1472,7 +1465,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1480,7 +1473,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1488,7 +1481,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1496,7 +1489,15 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1513,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1540,7 +1541,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1557,13 +1558,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -1581,10 +1582,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="9"/>
@@ -1603,7 +1604,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>12</v>
@@ -1625,10 +1626,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="9"/>
@@ -1647,10 +1648,10 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="9"/>
@@ -1669,10 +1670,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="9"/>
@@ -1691,10 +1692,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="9"/>
@@ -1713,10 +1714,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="9"/>
@@ -1735,10 +1736,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
@@ -1757,10 +1758,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
@@ -1779,10 +1780,10 @@
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9"/>
@@ -1801,10 +1802,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="9"/>
@@ -1823,10 +1824,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="12"/>
@@ -1845,10 +1846,10 @@
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1862,10 +1863,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1879,10 +1880,10 @@
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1896,321 +1897,321 @@
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C27" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="B28" s="2">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2">
         <v>6</v>
       </c>
-      <c r="C28" s="2">
-        <v>3</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C29" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C30" s="2">
         <v>3</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" s="2">
         <v>7</v>
       </c>
       <c r="C31" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2">
         <v>8</v>
       </c>
       <c r="C34" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="2">
         <v>8</v>
       </c>
       <c r="C35" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="2">
         <v>8</v>
       </c>
       <c r="C36" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B37" s="2">
         <v>8</v>
@@ -2219,134 +2220,134 @@
         <v>8</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C39" s="2">
         <v>8</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B40" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C40" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B41" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C41" s="2">
         <v>8</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>109</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C42" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B43" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B44" s="2">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C44" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B45" s="2">
         <v>13</v>
@@ -2355,117 +2356,117 @@
         <v>2</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B46" s="2">
         <v>13</v>
       </c>
       <c r="C46" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" s="2">
         <v>13</v>
       </c>
       <c r="C47" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B48" s="2">
         <v>13</v>
       </c>
       <c r="C48" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B49" s="2">
         <v>13</v>
       </c>
       <c r="C49" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B50" s="2">
         <v>13</v>
       </c>
       <c r="C50" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B51" s="2">
         <v>13</v>
       </c>
       <c r="C51" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B52" s="2">
         <v>13</v>
@@ -2474,15 +2475,15 @@
         <v>3</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B53" s="2">
         <v>13</v>
@@ -2491,15 +2492,15 @@
         <v>2</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B54" s="2">
         <v>13</v>
@@ -2508,49 +2509,49 @@
         <v>3</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B55" s="2">
         <v>13</v>
       </c>
       <c r="C55" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B56" s="2">
         <v>13</v>
       </c>
       <c r="C56" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B57" s="2">
         <v>13</v>
@@ -2559,49 +2560,49 @@
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B58" s="2">
         <v>13</v>
       </c>
       <c r="C58" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B59" s="2">
         <v>13</v>
       </c>
       <c r="C59" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B60" s="2">
         <v>13</v>
@@ -2610,83 +2611,83 @@
         <v>3</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B61" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C61" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B62" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C62" s="2">
         <v>3</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B63" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C63" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B64" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C64" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B65" s="2">
         <v>15</v>
@@ -2695,24 +2696,24 @@
         <v>7</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B66" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C66" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>103</v>
@@ -2720,58 +2721,92 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B67" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C67" s="2">
         <v>7</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B68" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C68" s="2">
         <v>3</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
+        <v>66</v>
+      </c>
+      <c r="B69" s="2">
+        <v>17</v>
+      </c>
+      <c r="C69" s="2">
+        <v>7</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>67</v>
+      </c>
+      <c r="B70" s="2">
+        <v>18</v>
+      </c>
+      <c r="C70" s="2">
+        <v>3</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
         <v>68</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B71" s="2">
         <v>19</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C71" s="2">
         <v>3</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>111</v>
+      <c r="D71" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" autoFilter="0"/>
-  <autoFilter ref="A1:E68" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}"/>
+  <sheetProtection autoFilter="0"/>
+  <autoFilter ref="A1:E70" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}"/>
   <mergeCells count="1">
     <mergeCell ref="J2:N14"/>
   </mergeCells>
@@ -2785,13 +2820,13 @@
           <x14:formula1>
             <xm:f>part!$A$2:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>B2 C4 B65:B1048576 B5:B63</xm:sqref>
+          <xm:sqref>B2 C4 B5:B65 B67:B71 B72:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DF41E39-455D-45E0-B4E4-591C933514BF}">
           <x14:formula1>
             <xm:f>character!$A$2:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>C2 C65:C1048576 C4:C63</xm:sqref>
+          <xm:sqref>C2 C4:C65 C67:C71 C72:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2838,7 +2873,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D2" s="2"/>
       <c r="I2" s="5" t="s">
@@ -2857,7 +2892,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2"/>
       <c r="I3" s="16"/>
@@ -2874,7 +2909,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D4" s="2"/>
       <c r="I4" s="16"/>
@@ -2891,7 +2926,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D5" s="2"/>
       <c r="I5" s="16"/>
@@ -3853,7 +3888,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B061150C-8AD1-4314-86B3-91E6C7AB40D6}">
           <x14:formula1>
-            <xm:f>dialog!$A$2:$A$1000</xm:f>
+            <xm:f>dialog!$A$2:$A$1001</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
@@ -3891,10 +3926,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -3932,7 +3967,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
@@ -3945,7 +3980,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
@@ -3971,7 +4006,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
@@ -3984,7 +4019,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>

</xml_diff>

<commit_message>
Rebuild field scene; Add new bgm, font and modified plenty of details;
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6910DC8D-C8B7-4AF5-9DCE-45273E954ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D9AC11-DD1E-4848-B0FE-105C1CDBFE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
   <sheets>
     <sheet name="part" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="116">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -683,10 +683,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>你怎么能用假币买东西呢！</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>这是一张真钱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -724,6 +720,22 @@
   </si>
   <si>
     <t>跟娘去把水稻插上，猪给喂咯。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你怎么给我假钱！（怒）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>啊？是假钱吗？让我看看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>啊，好像还真是诶。不好意思，但是我也没有带别的钱了，不然我把这个给你吧！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（获得隐藏物品！请打开背包查看）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1266,18 +1278,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B08BA5-9D33-400C-B73F-DB35ECCAFF73}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.875" style="3"/>
+    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1285,7 +1297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1300,7 +1312,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1313,7 +1325,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1326,7 +1338,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1339,21 +1351,21 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1366,7 +1378,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1379,7 +1391,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1392,7 +1404,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1405,7 +1417,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1418,7 +1430,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1431,7 +1443,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1444,7 +1456,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1452,7 +1464,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1460,7 +1472,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1468,7 +1480,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1476,7 +1488,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1484,20 +1496,20 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1514,23 +1526,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N71"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="97" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.875" style="3"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1571,7 +1583,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1593,7 +1605,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1615,7 +1627,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1629,7 +1641,7 @@
         <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="9"/>
@@ -1637,7 +1649,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1659,7 +1671,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1681,7 +1693,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1703,7 +1715,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1725,7 +1737,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1747,7 +1759,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1769,7 +1781,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1791,7 +1803,7 @@
       <c r="M12" s="9"/>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1813,7 +1825,7 @@
       <c r="M13" s="9"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1835,7 +1847,7 @@
       <c r="M14" s="12"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1869,7 +1881,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1886,7 +1898,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1903,7 +1915,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>69</v>
       </c>
@@ -1917,10 +1929,10 @@
         <v>41</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1937,7 +1949,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1954,7 +1966,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1971,7 +1983,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -1988,7 +2000,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2005,7 +2017,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2022,7 +2034,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2039,7 +2051,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2056,7 +2068,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>70</v>
       </c>
@@ -2070,10 +2082,10 @@
         <v>41</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -2090,7 +2102,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -2107,7 +2119,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -2124,7 +2136,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -2141,7 +2153,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -2158,7 +2170,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -2175,7 +2187,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -2192,7 +2204,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -2209,7 +2221,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -2226,7 +2238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -2243,7 +2255,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -2257,10 +2269,10 @@
         <v>41</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -2277,7 +2289,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -2294,7 +2306,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -2311,7 +2323,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -2325,10 +2337,10 @@
         <v>41</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -2345,7 +2357,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -2362,7 +2374,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -2379,7 +2391,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -2396,7 +2408,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -2413,7 +2425,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -2430,7 +2442,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>47</v>
       </c>
@@ -2447,7 +2459,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>48</v>
       </c>
@@ -2464,7 +2476,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>49</v>
       </c>
@@ -2481,7 +2493,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>50</v>
       </c>
@@ -2498,7 +2510,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>51</v>
       </c>
@@ -2515,7 +2527,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>52</v>
       </c>
@@ -2532,7 +2544,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>53</v>
       </c>
@@ -2549,7 +2561,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>54</v>
       </c>
@@ -2566,7 +2578,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>55</v>
       </c>
@@ -2583,7 +2595,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>56</v>
       </c>
@@ -2600,7 +2612,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>57</v>
       </c>
@@ -2617,7 +2629,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>58</v>
       </c>
@@ -2634,7 +2646,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>59</v>
       </c>
@@ -2651,7 +2663,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>60</v>
       </c>
@@ -2668,7 +2680,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>61</v>
       </c>
@@ -2685,7 +2697,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>62</v>
       </c>
@@ -2702,7 +2714,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>63</v>
       </c>
@@ -2716,10 +2728,10 @@
         <v>41</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>64</v>
       </c>
@@ -2736,7 +2748,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>65</v>
       </c>
@@ -2753,7 +2765,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>66</v>
       </c>
@@ -2770,7 +2782,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>67</v>
       </c>
@@ -2784,24 +2796,75 @@
         <v>41</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
+        <v>71</v>
+      </c>
+      <c r="B71" s="2">
+        <v>18</v>
+      </c>
+      <c r="C71" s="2">
+        <v>8</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>72</v>
+      </c>
+      <c r="B72" s="2">
+        <v>18</v>
+      </c>
+      <c r="C72" s="2">
+        <v>8</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>73</v>
+      </c>
+      <c r="B73" s="2">
+        <v>18</v>
+      </c>
+      <c r="C73" s="2">
+        <v>7</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
         <v>68</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B74" s="2">
         <v>19</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C74" s="2">
         <v>3</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>108</v>
+      <c r="D74" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2820,13 +2883,13 @@
           <x14:formula1>
             <xm:f>part!$A$2:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>B2 C4 B5:B65 B67:B71 B72:B1048576</xm:sqref>
+          <xm:sqref>B2 C4 B5:B65 B67:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DF41E39-455D-45E0-B4E4-591C933514BF}">
           <x14:formula1>
             <xm:f>character!$A$2:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>C2 C4:C65 C67:C71 C72:C1048576</xm:sqref>
+          <xm:sqref>C2 C4:C65 C67:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2842,16 +2905,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.875" style="3"/>
+    <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2865,7 +2928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2884,7 +2947,7 @@
       <c r="L2" s="14"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2892,7 +2955,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="2"/>
       <c r="I3" s="16"/>
@@ -2901,7 +2964,7 @@
       <c r="L3" s="17"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2918,7 +2981,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2935,7 +2998,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2946,7 +3009,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2957,7 +3020,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2968,7 +3031,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2979,7 +3042,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2990,7 +3053,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3001,7 +3064,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3012,7 +3075,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3023,7 +3086,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3034,7 +3097,7 @@
       <c r="L14" s="17"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3045,7 +3108,7 @@
       <c r="L15" s="17"/>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3056,7 +3119,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3067,7 +3130,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3078,793 +3141,793 @@
       <c r="L18" s="20"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3888,7 +3951,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B061150C-8AD1-4314-86B3-91E6C7AB40D6}">
           <x14:formula1>
-            <xm:f>dialog!$A$2:$A$1001</xm:f>
+            <xm:f>dialog!$A$2:$A$1000</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
@@ -3906,14 +3969,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.875" style="3"/>
+    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3921,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3936,7 +3999,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3949,7 +4012,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3962,7 +4025,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3975,7 +4038,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3988,7 +4051,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4001,7 +4064,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4014,7 +4077,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4027,35 +4090,35 @@
       <c r="J9" s="9"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>

</xml_diff>

<commit_message>
Add hint after plant at field
</commit_message>
<xml_diff>
--- a/Assets/Editors/Data/GameData.xlsx
+++ b/Assets/Editors/Data/GameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unity projects\Planet-Plant\Assets\Editors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D9AC11-DD1E-4848-B0FE-105C1CDBFE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FACE58-90AD-407F-A383-3CCC2523FBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1EAA04EB-E6EE-47C2-942C-AC0C5B2D7D63}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -736,6 +736,14 @@
   </si>
   <si>
     <t>（获得隐藏物品！请打开背包查看）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一天种完地回家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>终于种好了，差不多也该回家吃午饭了。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1279,7 +1287,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1352,6 +1360,12 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -1526,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D23B0CC-53CD-46B8-9128-2C88785E85DC}">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2865,6 +2879,23 @@
       </c>
       <c r="E74" s="2" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2">
+        <v>5</v>
+      </c>
+      <c r="C75" s="2">
+        <v>3</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>